<commit_message>
revised the title of the related manuscript
</commit_message>
<xml_diff>
--- a/EWU_Dashboard_InputTemplate.xlsx
+++ b/EWU_Dashboard_InputTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahSchmidt\Documents\sourcetree\MoEWe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D442DB-1C37-44D4-9D03-EC150A5C10E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF721D0-FE4E-4663-8A58-8DD31601FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1006,7 +1006,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="620">
   <si>
     <t>input</t>
   </si>
@@ -3274,6 +3274,9 @@
   </si>
   <si>
     <t>Weighting factors are used to aggregate impact category wise calculated impacts and indicator scores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schmidt, S.; Laner, D. (in preparation): Environmental Waste Utilization score to monitor the performance of waste management systems: A novel indicator applied to case studies in Germany </t>
   </si>
 </sst>
 </file>
@@ -3622,7 +3625,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3769,6 +3772,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5060,7 +5066,9 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5099,11 +5107,11 @@
       </c>
       <c r="B6" s="73"/>
     </row>
-    <row r="7" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="74" t="s">
-        <v>608</v>
-      </c>
-      <c r="B7" s="73"/>
+    <row r="7" spans="1:2" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="78" t="s">
+        <v>619</v>
+      </c>
+      <c r="B7" s="78"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
@@ -5210,8 +5218,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>